<commit_message>
Ajout ci-build message 40e73818b405ab3cd55ea5bdf7793eae299a4c02
</commit_message>
<xml_diff>
--- a/nriss-patch-1/ig/PN13-FHIR-TypoComposant-conceptmap.xlsx
+++ b/nriss-patch-1/ig/PN13-FHIR-TypoComposant-conceptmap.xlsx
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-09-18T09:12:00+00:00</t>
+    <t>2025-04-10T15:35:36+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -99,7 +99,7 @@
     <t>Target</t>
   </si>
   <si>
-    <t>https://hl7.fr/ig/fhir/Medication/CodeSystem/fr-medication-profil-list</t>
+    <t>https://hl7.fr/fhir/fr/medication/CodeSystem/fr-medication-profile-list</t>
   </si>
   <si>
     <t>Display</t>

</xml_diff>